<commit_message>
Updated chart and readme
</commit_message>
<xml_diff>
--- a/Budget_tmp1.xlsx
+++ b/Budget_tmp1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HELIOS\Documents\0-CODE_BASE\DATA_PROJECTS\EXCEL\finance_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1E2EFF-5440-4B4C-AB01-37A940B508A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12447853-412C-4D09-B39F-DCAB0890945B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23835" yWindow="13380" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,12 +113,6 @@
     <t>TOTAL</t>
   </si>
   <si>
-    <t>Monthly_Bill_Amount</t>
-  </si>
-  <si>
-    <t>Split_Bill_Amount</t>
-  </si>
-  <si>
     <t>TOTAL NET INCOME:</t>
   </si>
   <si>
@@ -129,6 +123,12 @@
   </si>
   <si>
     <t>MONTHLY (BUDGET - BILLS):</t>
+  </si>
+  <si>
+    <t>Total_Bill_Amount</t>
+  </si>
+  <si>
+    <t>True_Bill_Deduction</t>
   </si>
 </sst>
 </file>
@@ -474,14 +474,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color auto="1"/>
-        </left>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -505,6 +497,14 @@
           <color auto="1"/>
         </left>
         <right/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color auto="1"/>
+        </left>
         <vertical/>
       </border>
     </dxf>
@@ -565,15 +565,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D3A6DA2C-FA75-487D-9539-4B84E11AF7E4}" name="Table223" displayName="Table223" ref="B3:I34" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
   <autoFilter ref="B3:I34" xr:uid="{D3A6DA2C-FA75-487D-9539-4B84E11AF7E4}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{5C1E4F42-C994-4043-8562-BF53677C9B58}" name="Source" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{15BF8101-832E-417C-8D3D-710128CEEAE4}" name="Type" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{5C1E4F42-C994-4043-8562-BF53677C9B58}" name="Source" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{15BF8101-832E-417C-8D3D-710128CEEAE4}" name="Type" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{A26B43F6-9438-45F5-B7AB-221CB6016DB8}" name="Active"/>
     <tableColumn id="4" xr3:uid="{313E200D-6869-402B-8575-49DDEB584AAC}" name="Split"/>
-    <tableColumn id="5" xr3:uid="{ABDDB1DE-1EDF-4BD7-A017-5E5E5D7D2AE0}" name="Monthly_Bill_Amount" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F3D68882-148C-4090-8835-6BCC9142114F}" name="Split_Bill_Amount" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{ABDDB1DE-1EDF-4BD7-A017-5E5E5D7D2AE0}" name="Total_Bill_Amount" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{F3D68882-148C-4090-8835-6BCC9142114F}" name="True_Bill_Deduction" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(D4="YES",IF(E4="YES",F4/2,F4), F4-F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C20E245B-BC47-4A6D-BF72-5E317BAC1765}" name="TAXES" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="9" xr3:uid="{C20E245B-BC47-4A6D-BF72-5E317BAC1765}" name="TAXES" dataDxfId="1" dataCellStyle="Percent"/>
     <tableColumn id="7" xr3:uid="{0DD8E2D7-1BE8-44E0-A868-63C5F0DC6739}" name="Monthly_Remaining" dataDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +856,7 @@
     <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="29.85546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="9" max="9" width="29.140625" customWidth="1"/>
   </cols>
@@ -871,11 +871,11 @@
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
       <c r="G2" s="33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H2" s="26"/>
       <c r="I2" s="40" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="24" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -892,10 +892,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>12</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -974,7 +974,7 @@
     </row>
     <row r="8" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>24</v>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="37">
-        <f>SUM(I8-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I8-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1019,7 +1019,7 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="38">
-        <f>SUM(I9-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I9-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="38">
-        <f>SUM(I10-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I10-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="38">
-        <f>SUM(I11-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I11-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="38">
-        <f>SUM(I12-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I12-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1089,7 +1089,7 @@
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="38">
-        <f>SUM(I13-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I13-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1107,7 +1107,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="38">
-        <f>SUM(I14-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I14-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="38">
-        <f>SUM(I15-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I15-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="38">
-        <f>SUM(I16-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I16-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="38">
-        <f>SUM(I17-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I17-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="38">
-        <f>SUM(I18-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I18-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="38">
-        <f>SUM(I19-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I19-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="38">
-        <f>SUM(I20-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I20-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="38">
-        <f>SUM(I21-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I21-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1249,7 +1249,7 @@
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="38">
-        <f>SUM(I22-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I22-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="38">
-        <f>SUM(I23-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I23-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="38">
-        <f>SUM(I24-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I24-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="H26" s="19"/>
       <c r="I26" s="38">
-        <f>SUM(I25-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I25-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="H27" s="19"/>
       <c r="I27" s="38">
-        <f>SUM(I26-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I26-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="38">
-        <f>SUM(I27-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I27-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="H29" s="19"/>
       <c r="I29" s="38">
-        <f>SUM(I28-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I28-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="38">
-        <f>SUM(I29-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I29-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="H31" s="19"/>
       <c r="I31" s="38">
-        <f>SUM(I30-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I30-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1401,7 +1401,7 @@
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="38">
-        <f>SUM(I31-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I31-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1417,13 +1417,13 @@
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="38">
-        <f>SUM(I32-Table223[[#This Row],[Split_Bill_Amount]])</f>
+        <f>SUM(I32-Table223[[#This Row],[True_Bill_Deduction]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>24</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="35" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E34" xr:uid="{C185138C-4223-4AA3-A14B-88D21360567B}">
       <formula1>"YES, NO"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
updated charts, readme, and tmpl
</commit_message>
<xml_diff>
--- a/Budget_tmp1.xlsx
+++ b/Budget_tmp1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HELIOS\Documents\0-CODE_BASE\DATA_PROJECTS\EXCEL\finance_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12447853-412C-4D09-B39F-DCAB0890945B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1C7986-20B5-4AEF-9BD2-8432F6B4A701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23835" yWindow="13380" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>MONTHLY EXPENSES AND INCOME TABLE</t>
   </si>
@@ -125,10 +125,13 @@
     <t>MONTHLY (BUDGET - BILLS):</t>
   </si>
   <si>
-    <t>Total_Bill_Amount</t>
-  </si>
-  <si>
-    <t>True_Bill_Deduction</t>
+    <t>CAR FINANCE</t>
+  </si>
+  <si>
+    <t>Total_Amount</t>
+  </si>
+  <si>
+    <t>True_Amount</t>
   </si>
 </sst>
 </file>
@@ -562,15 +565,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D3A6DA2C-FA75-487D-9539-4B84E11AF7E4}" name="Table223" displayName="Table223" ref="B3:I34" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
-  <autoFilter ref="B3:I34" xr:uid="{D3A6DA2C-FA75-487D-9539-4B84E11AF7E4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D3A6DA2C-FA75-487D-9539-4B84E11AF7E4}" name="Table223" displayName="Table223" ref="B3:I35" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4">
+  <autoFilter ref="B3:I35" xr:uid="{D3A6DA2C-FA75-487D-9539-4B84E11AF7E4}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5C1E4F42-C994-4043-8562-BF53677C9B58}" name="Source" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{15BF8101-832E-417C-8D3D-710128CEEAE4}" name="Type" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{A26B43F6-9438-45F5-B7AB-221CB6016DB8}" name="Active"/>
     <tableColumn id="4" xr3:uid="{313E200D-6869-402B-8575-49DDEB584AAC}" name="Split"/>
-    <tableColumn id="5" xr3:uid="{ABDDB1DE-1EDF-4BD7-A017-5E5E5D7D2AE0}" name="Total_Bill_Amount" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{F3D68882-148C-4090-8835-6BCC9142114F}" name="True_Bill_Deduction" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{ABDDB1DE-1EDF-4BD7-A017-5E5E5D7D2AE0}" name="Total_Amount" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{F3D68882-148C-4090-8835-6BCC9142114F}" name="True_Amount" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(D4="YES",IF(E4="YES",F4/2,F4), F4-F4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{C20E245B-BC47-4A6D-BF72-5E317BAC1765}" name="TAXES" dataDxfId="1" dataCellStyle="Percent"/>
@@ -843,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I35"/>
+  <dimension ref="B1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,10 +895,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>12</v>
@@ -1003,7 +1006,7 @@
       </c>
       <c r="H9" s="18"/>
       <c r="I9" s="37">
-        <f>SUM(I8-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I8-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1019,7 +1022,7 @@
       </c>
       <c r="H10" s="19"/>
       <c r="I10" s="38">
-        <f>SUM(I9-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I9-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1030,12 +1033,12 @@
       <c r="E11" s="14"/>
       <c r="F11" s="1"/>
       <c r="G11" s="36">
-        <f t="shared" ref="G11:G33" si="0">IF(D11="YES",IF(E11="YES",F11/2,F11), F11-F11)</f>
+        <f t="shared" ref="G11:G34" si="0">IF(D11="YES",IF(E11="YES",F11/2,F11), F11-F11)</f>
         <v>0</v>
       </c>
       <c r="H11" s="19"/>
       <c r="I11" s="38">
-        <f>SUM(I10-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I10-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1053,7 +1056,7 @@
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="38">
-        <f>SUM(I11-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I11-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1071,7 +1074,7 @@
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="38">
-        <f>SUM(I12-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I12-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1089,7 +1092,7 @@
       </c>
       <c r="H14" s="19"/>
       <c r="I14" s="38">
-        <f>SUM(I13-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I13-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1107,7 +1110,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="38">
-        <f>SUM(I14-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I14-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1125,7 +1128,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="38">
-        <f>SUM(I15-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I15-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1143,7 +1146,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="38">
-        <f>SUM(I16-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I16-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1161,7 +1164,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="38">
-        <f>SUM(I17-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I17-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1179,7 +1182,7 @@
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="38">
-        <f>SUM(I18-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I18-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1195,7 +1198,7 @@
       </c>
       <c r="H20" s="19"/>
       <c r="I20" s="38">
-        <f>SUM(I19-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I19-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1213,7 +1216,7 @@
       </c>
       <c r="H21" s="19"/>
       <c r="I21" s="38">
-        <f>SUM(I20-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I20-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1231,31 +1234,31 @@
       </c>
       <c r="H22" s="19"/>
       <c r="I22" s="38">
-        <f>SUM(I21-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I21-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="14"/>
       <c r="F23" s="1"/>
       <c r="G23" s="35">
-        <f t="shared" si="0"/>
+        <f>IF(D23="YES",IF(E23="YES",F23/2,F23), F23-F23)</f>
         <v>0</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23" s="38">
-        <f>SUM(I22-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I22-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1267,23 +1270,25 @@
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="38">
-        <f>SUM(I23-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I23-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="3"/>
+      <c r="F25" s="1"/>
       <c r="G25" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="38">
-        <f>SUM(I24-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I24-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1292,18 +1297,18 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="3"/>
       <c r="G26" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H26" s="19"/>
       <c r="I26" s="38">
-        <f>SUM(I25-Table223[[#This Row],[True_Bill_Deduction]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>SUM(I25-Table223[[#This Row],[True_Amount]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -1315,49 +1320,47 @@
       </c>
       <c r="H27" s="19"/>
       <c r="I27" s="38">
-        <f>SUM(I26-Table223[[#This Row],[True_Bill_Deduction]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="2"/>
+        <f>SUM(I26-Table223[[#This Row],[True_Amount]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="1"/>
       <c r="G28" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="38">
-        <f>SUM(I27-Table223[[#This Row],[True_Bill_Deduction]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="1"/>
+        <f>SUM(I27-Table223[[#This Row],[True_Amount]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="2"/>
       <c r="G29" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H29" s="19"/>
       <c r="I29" s="38">
-        <f>SUM(I28-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I28-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1369,12 +1372,14 @@
       </c>
       <c r="H30" s="19"/>
       <c r="I30" s="38">
-        <f>SUM(I29-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I29-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="5"/>
+      <c r="B31" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="14"/>
@@ -1385,7 +1390,7 @@
       </c>
       <c r="H31" s="19"/>
       <c r="I31" s="38">
-        <f>SUM(I30-Table223[[#This Row],[True_Bill_Deduction]])</f>
+        <f>SUM(I30-Table223[[#This Row],[True_Amount]])</f>
         <v>0</v>
       </c>
     </row>
@@ -1401,53 +1406,69 @@
       </c>
       <c r="H32" s="19"/>
       <c r="I32" s="38">
-        <f>SUM(I31-Table223[[#This Row],[True_Bill_Deduction]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>SUM(I31-Table223[[#This Row],[True_Amount]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="3"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="1"/>
       <c r="G33" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H33" s="20"/>
+      <c r="H33" s="19"/>
       <c r="I33" s="38">
-        <f>SUM(I32-Table223[[#This Row],[True_Bill_Deduction]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="21" t="s">
+        <f>SUM(I32-Table223[[#This Row],[True_Amount]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="20"/>
+      <c r="I34" s="38">
+        <f>SUM(I33-Table223[[#This Row],[True_Amount]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="21.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C35" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="42">
-        <f>SUM(G12:G33)</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="31"/>
-      <c r="I34" s="41">
-        <f>I33</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="42">
+        <f>SUM(G12:G34)</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="31"/>
+      <c r="I35" s="41">
+        <f>I34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E34" xr:uid="{C185138C-4223-4AA3-A14B-88D21360567B}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:E35" xr:uid="{C185138C-4223-4AA3-A14B-88D21360567B}">
       <formula1>"YES, NO"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C34" xr:uid="{38EC75DB-4AF9-4173-91AC-98FE4D44BB54}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C35" xr:uid="{38EC75DB-4AF9-4173-91AC-98FE4D44BB54}">
       <formula1>"Income, Savings, Essential-bill, Non-essential-bill, Loan, Expense, TOTAL"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>